<commit_message>
Premium calculation for iBegin product
</commit_message>
<xml_diff>
--- a/documentation/Calculate_Sheet_iBegin V.01.xlsx
+++ b/documentation/Calculate_Sheet_iBegin V.01.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\ALL\99 Projects\eBiz\Day1\Premuim &amp; CV (10EC, iBegin)\iBegin\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="655"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23540" windowHeight="14120" tabRatio="655"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate sheet (PRM)" sheetId="9" r:id="rId1"/>
     <sheet name="PremiumRate_iBegin" sheetId="10" r:id="rId2"/>
     <sheet name="Calculate Factor" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -31,7 +29,7 @@
     <author>Wiboon Oransirikul</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="272">
   <si>
     <t>Premium</t>
   </si>
@@ -884,11 +882,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;???_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,6 +922,24 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -962,42 +978,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1005,16 +1021,60 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1024,7 +1084,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1054,35 +1114,35 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1098,8 +1158,52 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="47">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -1159,7 +1263,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1194,7 +1298,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1371,7 +1475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1381,22 +1485,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.625" style="2" customWidth="1"/>
     <col min="5" max="7" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="3.875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="3.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="14.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1406,9 +1510,8 @@
       <c r="B1" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="2" t="str">
-        <f>IF(B1="Male","M","F")</f>
-        <v>M</v>
+      <c r="E1" s="2" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1416,12 +1519,12 @@
         <v>269</v>
       </c>
       <c r="B2" s="18">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C2" s="3"/>
       <c r="E2" s="2" t="str">
         <f>"S"&amp;C4&amp;"T"&amp;LEFT(B5,2)</f>
-        <v>S5T10</v>
+        <v>S5T20</v>
       </c>
       <c r="O2" s="2">
         <v>12.023</v>
@@ -1478,7 +1581,7 @@
         <v>270</v>
       </c>
       <c r="B5" s="20">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="O5" s="2">
         <v>12.323</v>
@@ -1494,7 +1597,7 @@
       </c>
       <c r="B6" s="19">
         <f>VLOOKUP(E2&amp;""&amp;E1,PremiumRate_iBegin!A1:CA29,'Calculate sheet (PRM)'!B2+9,FALSE)</f>
-        <v>365.07</v>
+        <v>423.66</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1506,7 +1609,7 @@
       </c>
       <c r="B7" s="23">
         <f>(B5*B6/1000)*C3</f>
-        <v>36507</v>
+        <v>84732</v>
       </c>
       <c r="O7" s="2">
         <v>12.423</v>
@@ -1569,7 +1672,7 @@
       </c>
       <c r="D12" s="15">
         <f>B7*1.02</f>
-        <v>37237.14</v>
+        <v>86426.64</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>244</v>
@@ -1595,7 +1698,7 @@
       </c>
       <c r="D13" s="15">
         <f>(B7*1.02)*2</f>
-        <v>74474.28</v>
+        <v>172853.28</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>245</v>
@@ -1621,7 +1724,7 @@
       </c>
       <c r="D14" s="15">
         <f>B5*1.15</f>
-        <v>114999.99999999999</v>
+        <v>229999.99999999997</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>246</v>
@@ -1640,7 +1743,7 @@
       </c>
       <c r="D15" s="15">
         <f>B5*1.3</f>
-        <v>130000</v>
+        <v>260000</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>247</v>
@@ -1659,7 +1762,7 @@
       </c>
       <c r="D16" s="15">
         <f>B5*1.5</f>
-        <v>150000</v>
+        <v>300000</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>248</v>
@@ -1694,7 +1797,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="16">
         <f>B5</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>252</v>
@@ -1707,7 +1810,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="16">
         <f>B5*0.005</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>253</v>
@@ -1767,7 +1870,7 @@
       </c>
       <c r="D26" s="13">
         <f>B5*0.1</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>254</v>
@@ -1782,7 +1885,7 @@
       </c>
       <c r="D27" s="13">
         <f>B5*0.15</f>
-        <v>15000</v>
+        <v>30000</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>255</v>
@@ -1797,7 +1900,7 @@
       </c>
       <c r="D28" s="13">
         <f>B5*0.25</f>
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>256</v>
@@ -1810,7 +1913,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="14">
         <f>B5*0.005</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>257</v>
@@ -1823,7 +1926,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="13">
         <f>(B7*B3)*C4</f>
-        <v>182535</v>
+        <v>423660</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>265</v>
@@ -1836,8 +1939,8 @@
     <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="80" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" scale="80" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -1861,6 +1964,9 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -1876,9 +1982,9 @@
       <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="16384" width="9.125" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:208">
@@ -20069,6 +20175,11 @@
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -20080,10 +20191,10 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -20173,5 +20284,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>